<commit_message>
add employee saving and fix joint saving
</commit_message>
<xml_diff>
--- a/uploads/data/contoh_format_excel_joint.xlsx
+++ b/uploads/data/contoh_format_excel_joint.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\keuangan\uploads\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC20742-FD2D-4D49-9E89-458D02C63A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4FBE4F-1C61-4CDB-AC8C-ED07D15E90D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="768" windowWidth="23040" windowHeight="11364" xr2:uid="{0EA281BF-02DB-492B-900F-DF763AB3E8E2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{0EA281BF-02DB-492B-900F-DF763AB3E8E2}"/>
   </bookViews>
   <sheets>
     <sheet name="contoh_format_excel" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>TINGKAT</t>
   </si>
@@ -43,24 +43,12 @@
     <t>SD</t>
   </si>
   <si>
-    <t>SMP</t>
-  </si>
-  <si>
-    <t>KB</t>
-  </si>
-  <si>
     <t>BAISAH</t>
   </si>
   <si>
-    <t>DAISAH</t>
-  </si>
-  <si>
     <t>08977665545</t>
   </si>
   <si>
-    <t>08977665548</t>
-  </si>
-  <si>
     <t>NOMOR_REKENING_BERSAMA</t>
   </si>
   <si>
@@ -70,24 +58,6 @@
     <t>SALDO_BERSAMA</t>
   </si>
   <si>
-    <t>NIS_PENANGGUNG_JAWAB</t>
-  </si>
-  <si>
-    <t>TABUNGAN1</t>
-  </si>
-  <si>
-    <t>TABUNGAN2</t>
-  </si>
-  <si>
-    <t>TABUNGAN3</t>
-  </si>
-  <si>
-    <t>TABUNGAN4</t>
-  </si>
-  <si>
-    <t>TABUNGAN5</t>
-  </si>
-  <si>
     <r>
       <t>*untuk format isian kolom</t>
     </r>
@@ -137,17 +107,249 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>NIS_PENANGGUNG_JAWAB,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> NIS harus sudah </t>
+      <t xml:space="preserve">NOMOR_REKENING_BERSAMA </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">wajib 7 karakter angka </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(WAJIB DI ISI)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">*untuk format isian kolom </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NAMA_TABUNGAN_BERSAMA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> gunakan karakter biasa </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(WAJIB DI ISI)</t>
+    </r>
+  </si>
+  <si>
+    <t>JENIS_TABUNGAN</t>
+  </si>
+  <si>
+    <t>KOMITE</t>
+  </si>
+  <si>
+    <t>KELAS</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">*untuk format isian kolom </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>JENIS_TABUNGAN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> wajib diisi </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(KOMITE/KELAS)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tanpa tambahan kata </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(WAJIB DI ISI)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">*untuk format isian kolom </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TINGKAT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> wajib diisi </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(DC/KB/TK/SD/SMP)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> tanpa ICP dll </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(WAJIB DI ISI)</t>
+    </r>
+  </si>
+  <si>
+    <t>TABUNGAN KOMITE TK</t>
+  </si>
+  <si>
+    <t>TABUNGAN KELAS TK A</t>
+  </si>
+  <si>
+    <t>TABUNGAN KOMITE SD</t>
+  </si>
+  <si>
+    <t>NOMOR_PENANGGUNG_JAWAB</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">*untuk format isian kolom </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOMOR_PENANGGUNG_JAWAB,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NIP/NIS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> harus sudah </t>
     </r>
     <r>
       <rPr>
@@ -168,7 +370,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> di nasabah personal </t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
@@ -184,166 +386,55 @@
   </si>
   <si>
     <r>
+      <t>*untuk format isian kolom</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> NAMA_WALI, NOMOR_HP_WALI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">tidak wajib di isi, "kosongkan jika tidak ada" </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(TIDAK WAJIB DI ISI)</t>
+    </r>
+  </si>
+  <si>
+    <t>089776655</t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">*untuk format isian kolom </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>TINGKAT</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> wajib (DC/KB/TK/SD/SMP) tanpa ICP dll </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(WAJIB DI ISI)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>*untuk format isian kolom</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> NAMA_WALI, NOMOR_HP_WALI </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">tidak wajib di isi, "kosongkan" </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(TIDAK WAJIB DI ISI)</t>
-    </r>
-  </si>
-  <si>
-    <t>DC</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">*untuk format isian kolom </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">NOMOR_REKENING_BERSAMA </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">wajib 7 karakter angka </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(WAJIB DI ISI)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">*untuk format isian kolom </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>NAMA_TABUNGAN_BERSAMA</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> gunakan karakter biasa </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(WAJIB DI ISI)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">*untuk format isian kolom </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
         <color theme="1"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">NOMOR _HP_WALI  </t>
+      <t xml:space="preserve">NOMOR _HP_WALI </t>
     </r>
     <r>
       <rPr>
@@ -1294,36 +1385,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AA0F0B5-3F2A-41A4-B914-484C0C045741}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="97.77734375" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="100.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>0</v>
@@ -1333,20 +1425,23 @@
       </c>
       <c r="G1" s="4" t="s">
         <v>2</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
+        <v>2200333</v>
+      </c>
+      <c r="B2">
         <v>123456</v>
       </c>
-      <c r="B2">
-        <v>12345</v>
-      </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>500000</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -1356,115 +1451,96 @@
       </c>
       <c r="G2" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>123457</v>
+        <v>1234567</v>
       </c>
       <c r="B3">
         <v>123457</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D3">
         <v>100000</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>123458</v>
+        <v>2200344</v>
       </c>
       <c r="B4">
         <v>123458</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
         <v>7</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
       <c r="J4" s="2" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>123459</v>
-      </c>
-      <c r="B5">
-        <v>123459</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5">
-        <v>500000</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
       <c r="J5" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>123460</v>
-      </c>
-      <c r="B6">
-        <v>123460</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6">
-        <v>700000</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="J6" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J7" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J8" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J9" s="5" t="s">
-        <v>25</v>
+      <c r="J9" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J10" t="s">
-        <v>29</v>
+      <c r="J10" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J11" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>